<commit_message>
no se que hizo lizz
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14580" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz" sheetId="1" r:id="rId1"/>
     <sheet name="Entrenamiento" sheetId="2" r:id="rId2"/>
     <sheet name="Analisis" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:AJ29"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25:AH25"/>
+      <selection activeCell="AI17" sqref="AI17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3114,7 +3114,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>